<commit_message>
add monthly report and change date wokers
</commit_message>
<xml_diff>
--- a/blank/monthly.xlsx
+++ b/blank/monthly.xlsx
@@ -37,7 +37,7 @@
     <t xml:space="preserve">Состав проведенных работ</t>
   </si>
   <si>
-    <t xml:space="preserve">Исполнитель</t>
+    <t xml:space="preserve">Исполнитель / подпись</t>
   </si>
   <si>
     <t xml:space="preserve">Подпись</t>
@@ -245,6 +245,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -265,11 +266,13 @@
       <sz val="14"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="12"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
@@ -294,7 +297,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="8">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -311,6 +314,13 @@
     </border>
     <border diagonalUp="false" diagonalDown="false">
       <left style="thin"/>
+      <right/>
+      <top style="thin"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
       <right style="thin"/>
       <top style="thin"/>
       <bottom/>
@@ -318,9 +328,30 @@
     </border>
     <border diagonalUp="false" diagonalDown="false">
       <left style="thin"/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
       <right style="thin"/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right/>
+      <top/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="thin"/>
+      <top/>
+      <bottom style="thin"/>
       <diagonal/>
     </border>
   </borders>
@@ -349,7 +380,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -362,11 +393,11 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -378,8 +409,8 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -390,7 +421,7 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -398,12 +429,40 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -425,15 +484,15 @@
   </sheetPr>
   <dimension ref="A1:F98"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A91" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I94" activeCellId="0" sqref="I94"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G8" activeCellId="0" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="8.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="10.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="18.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="18.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="61.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="16.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="15.14"/>
@@ -470,7 +529,7 @@
       <c r="D3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="7" t="s">
         <v>5</v>
       </c>
       <c r="F3" s="7" t="s">
@@ -496,16 +555,16 @@
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
       <c r="D5" s="9"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="11"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="13"/>
     </row>
     <row r="6" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="8"/>
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
       <c r="D6" s="9"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="11"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="15"/>
     </row>
     <row r="7" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="8"/>
@@ -518,7 +577,7 @@
       <c r="D7" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="12"/>
+      <c r="E7" s="16"/>
       <c r="F7" s="11"/>
     </row>
     <row r="8" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -526,16 +585,16 @@
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
       <c r="D8" s="9"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="11"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="13"/>
     </row>
     <row r="9" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="8"/>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
       <c r="D9" s="9"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="11"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="15"/>
     </row>
     <row r="10" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="8"/>
@@ -548,7 +607,7 @@
       <c r="D10" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="12"/>
+      <c r="E10" s="16"/>
       <c r="F10" s="11"/>
     </row>
     <row r="11" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -556,16 +615,16 @@
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
       <c r="D11" s="9"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="11"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="13"/>
     </row>
     <row r="12" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="8"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
       <c r="D12" s="9"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="11"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="15"/>
     </row>
     <row r="13" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="8"/>
@@ -578,7 +637,7 @@
       <c r="D13" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="E13" s="12"/>
+      <c r="E13" s="16"/>
       <c r="F13" s="11"/>
     </row>
     <row r="14" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -586,16 +645,16 @@
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
       <c r="D14" s="9"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="11"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="13"/>
     </row>
     <row r="15" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="8"/>
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
       <c r="D15" s="9"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="11"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="15"/>
     </row>
     <row r="16" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="8"/>
@@ -608,7 +667,7 @@
       <c r="D16" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="E16" s="12"/>
+      <c r="E16" s="16"/>
       <c r="F16" s="11"/>
     </row>
     <row r="17" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -616,16 +675,16 @@
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
       <c r="D17" s="9"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="11"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="13"/>
     </row>
     <row r="18" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="8"/>
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
       <c r="D18" s="9"/>
-      <c r="E18" s="12"/>
-      <c r="F18" s="11"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="15"/>
     </row>
     <row r="19" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="8"/>
@@ -638,7 +697,7 @@
       <c r="D19" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="E19" s="12"/>
+      <c r="E19" s="16"/>
       <c r="F19" s="11"/>
     </row>
     <row r="20" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -646,16 +705,16 @@
       <c r="B20" s="6"/>
       <c r="C20" s="6"/>
       <c r="D20" s="9"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="11"/>
+      <c r="E20" s="17"/>
+      <c r="F20" s="13"/>
     </row>
     <row r="21" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="8"/>
       <c r="B21" s="6"/>
       <c r="C21" s="6"/>
       <c r="D21" s="9"/>
-      <c r="E21" s="12"/>
-      <c r="F21" s="11"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="15"/>
     </row>
     <row r="22" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="8"/>
@@ -668,7 +727,7 @@
       <c r="D22" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="E22" s="12"/>
+      <c r="E22" s="16"/>
       <c r="F22" s="11"/>
     </row>
     <row r="23" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -676,16 +735,16 @@
       <c r="B23" s="6"/>
       <c r="C23" s="6"/>
       <c r="D23" s="9"/>
-      <c r="E23" s="12"/>
-      <c r="F23" s="11"/>
+      <c r="E23" s="17"/>
+      <c r="F23" s="13"/>
     </row>
     <row r="24" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="8"/>
       <c r="B24" s="6"/>
       <c r="C24" s="6"/>
       <c r="D24" s="9"/>
-      <c r="E24" s="12"/>
-      <c r="F24" s="11"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="15"/>
     </row>
     <row r="25" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="8"/>
@@ -698,7 +757,7 @@
       <c r="D25" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="E25" s="12"/>
+      <c r="E25" s="16"/>
       <c r="F25" s="11"/>
     </row>
     <row r="26" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -706,16 +765,16 @@
       <c r="B26" s="6"/>
       <c r="C26" s="6"/>
       <c r="D26" s="9"/>
-      <c r="E26" s="12"/>
-      <c r="F26" s="11"/>
+      <c r="E26" s="17"/>
+      <c r="F26" s="13"/>
     </row>
     <row r="27" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="8"/>
       <c r="B27" s="6"/>
       <c r="C27" s="6"/>
       <c r="D27" s="9"/>
-      <c r="E27" s="12"/>
-      <c r="F27" s="11"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="15"/>
     </row>
     <row r="28" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="8"/>
@@ -728,7 +787,7 @@
       <c r="D28" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="E28" s="12"/>
+      <c r="E28" s="16"/>
       <c r="F28" s="11"/>
     </row>
     <row r="29" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -736,16 +795,16 @@
       <c r="B29" s="6"/>
       <c r="C29" s="6"/>
       <c r="D29" s="9"/>
-      <c r="E29" s="12"/>
-      <c r="F29" s="11"/>
+      <c r="E29" s="17"/>
+      <c r="F29" s="13"/>
     </row>
     <row r="30" customFormat="false" ht="61.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="8"/>
       <c r="B30" s="6"/>
       <c r="C30" s="6"/>
       <c r="D30" s="9"/>
-      <c r="E30" s="12"/>
-      <c r="F30" s="11"/>
+      <c r="E30" s="18"/>
+      <c r="F30" s="15"/>
     </row>
     <row r="31" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="8"/>
@@ -758,7 +817,7 @@
       <c r="D31" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="E31" s="12"/>
+      <c r="E31" s="16"/>
       <c r="F31" s="11"/>
     </row>
     <row r="32" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -766,16 +825,16 @@
       <c r="B32" s="6"/>
       <c r="C32" s="6"/>
       <c r="D32" s="9"/>
-      <c r="E32" s="12"/>
-      <c r="F32" s="11"/>
+      <c r="E32" s="17"/>
+      <c r="F32" s="13"/>
     </row>
     <row r="33" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="8"/>
       <c r="B33" s="6"/>
       <c r="C33" s="6"/>
       <c r="D33" s="9"/>
-      <c r="E33" s="12"/>
-      <c r="F33" s="11"/>
+      <c r="E33" s="18"/>
+      <c r="F33" s="15"/>
     </row>
     <row r="34" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="8"/>
@@ -788,7 +847,7 @@
       <c r="D34" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="E34" s="12"/>
+      <c r="E34" s="16"/>
       <c r="F34" s="11"/>
     </row>
     <row r="35" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -796,16 +855,16 @@
       <c r="B35" s="6"/>
       <c r="C35" s="6"/>
       <c r="D35" s="9"/>
-      <c r="E35" s="12"/>
-      <c r="F35" s="11"/>
+      <c r="E35" s="17"/>
+      <c r="F35" s="13"/>
     </row>
     <row r="36" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="8"/>
       <c r="B36" s="6"/>
       <c r="C36" s="6"/>
       <c r="D36" s="9"/>
-      <c r="E36" s="12"/>
-      <c r="F36" s="11"/>
+      <c r="E36" s="18"/>
+      <c r="F36" s="15"/>
     </row>
     <row r="37" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="8"/>
@@ -818,7 +877,7 @@
       <c r="D37" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="E37" s="12"/>
+      <c r="E37" s="16"/>
       <c r="F37" s="11"/>
     </row>
     <row r="38" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -826,16 +885,16 @@
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
       <c r="D38" s="9"/>
-      <c r="E38" s="12"/>
-      <c r="F38" s="11"/>
+      <c r="E38" s="17"/>
+      <c r="F38" s="13"/>
     </row>
     <row r="39" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="8"/>
       <c r="B39" s="6"/>
       <c r="C39" s="6"/>
       <c r="D39" s="9"/>
-      <c r="E39" s="12"/>
-      <c r="F39" s="11"/>
+      <c r="E39" s="18"/>
+      <c r="F39" s="15"/>
     </row>
     <row r="40" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="8"/>
@@ -848,7 +907,7 @@
       <c r="D40" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="E40" s="12"/>
+      <c r="E40" s="16"/>
       <c r="F40" s="11"/>
     </row>
     <row r="41" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -856,16 +915,16 @@
       <c r="B41" s="6"/>
       <c r="C41" s="6"/>
       <c r="D41" s="9"/>
-      <c r="E41" s="12"/>
-      <c r="F41" s="11"/>
+      <c r="E41" s="17"/>
+      <c r="F41" s="13"/>
     </row>
     <row r="42" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="8"/>
       <c r="B42" s="6"/>
       <c r="C42" s="6"/>
       <c r="D42" s="9"/>
-      <c r="E42" s="12"/>
-      <c r="F42" s="11"/>
+      <c r="E42" s="18"/>
+      <c r="F42" s="15"/>
     </row>
     <row r="43" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="8"/>
@@ -878,7 +937,7 @@
       <c r="D43" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="E43" s="12"/>
+      <c r="E43" s="16"/>
       <c r="F43" s="11"/>
     </row>
     <row r="44" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -886,16 +945,16 @@
       <c r="B44" s="6"/>
       <c r="C44" s="6"/>
       <c r="D44" s="9"/>
-      <c r="E44" s="12"/>
-      <c r="F44" s="11"/>
+      <c r="E44" s="17"/>
+      <c r="F44" s="13"/>
     </row>
     <row r="45" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="8"/>
       <c r="B45" s="6"/>
       <c r="C45" s="6"/>
       <c r="D45" s="9"/>
-      <c r="E45" s="12"/>
-      <c r="F45" s="11"/>
+      <c r="E45" s="18"/>
+      <c r="F45" s="15"/>
     </row>
     <row r="46" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="8"/>
@@ -908,7 +967,7 @@
       <c r="D46" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="E46" s="12"/>
+      <c r="E46" s="16"/>
       <c r="F46" s="11"/>
     </row>
     <row r="47" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -916,16 +975,16 @@
       <c r="B47" s="6"/>
       <c r="C47" s="6"/>
       <c r="D47" s="9"/>
-      <c r="E47" s="12"/>
-      <c r="F47" s="11"/>
+      <c r="E47" s="17"/>
+      <c r="F47" s="13"/>
     </row>
     <row r="48" customFormat="false" ht="135.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="8"/>
       <c r="B48" s="6"/>
       <c r="C48" s="6"/>
       <c r="D48" s="9"/>
-      <c r="E48" s="12"/>
-      <c r="F48" s="11"/>
+      <c r="E48" s="18"/>
+      <c r="F48" s="15"/>
     </row>
     <row r="49" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="8"/>
@@ -938,7 +997,7 @@
       <c r="D49" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="E49" s="12"/>
+      <c r="E49" s="16"/>
       <c r="F49" s="11"/>
     </row>
     <row r="50" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -946,16 +1005,16 @@
       <c r="B50" s="6"/>
       <c r="C50" s="6"/>
       <c r="D50" s="9"/>
-      <c r="E50" s="12"/>
-      <c r="F50" s="11"/>
+      <c r="E50" s="17"/>
+      <c r="F50" s="13"/>
     </row>
     <row r="51" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="8"/>
       <c r="B51" s="6"/>
       <c r="C51" s="6"/>
       <c r="D51" s="9"/>
-      <c r="E51" s="12"/>
-      <c r="F51" s="11"/>
+      <c r="E51" s="18"/>
+      <c r="F51" s="15"/>
     </row>
     <row r="52" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="8"/>
@@ -968,7 +1027,7 @@
       <c r="D52" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="E52" s="12"/>
+      <c r="E52" s="16"/>
       <c r="F52" s="11"/>
     </row>
     <row r="53" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -976,16 +1035,16 @@
       <c r="B53" s="6"/>
       <c r="C53" s="6"/>
       <c r="D53" s="9"/>
-      <c r="E53" s="12"/>
-      <c r="F53" s="11"/>
+      <c r="E53" s="17"/>
+      <c r="F53" s="13"/>
     </row>
     <row r="54" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="8"/>
       <c r="B54" s="6"/>
       <c r="C54" s="6"/>
       <c r="D54" s="9"/>
-      <c r="E54" s="12"/>
-      <c r="F54" s="11"/>
+      <c r="E54" s="18"/>
+      <c r="F54" s="15"/>
     </row>
     <row r="55" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="8"/>
@@ -998,7 +1057,7 @@
       <c r="D55" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="E55" s="12"/>
+      <c r="E55" s="16"/>
       <c r="F55" s="11"/>
     </row>
     <row r="56" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1006,16 +1065,16 @@
       <c r="B56" s="6"/>
       <c r="C56" s="6"/>
       <c r="D56" s="9"/>
-      <c r="E56" s="12"/>
-      <c r="F56" s="11"/>
+      <c r="E56" s="17"/>
+      <c r="F56" s="13"/>
     </row>
     <row r="57" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="8"/>
       <c r="B57" s="6"/>
       <c r="C57" s="6"/>
       <c r="D57" s="9"/>
-      <c r="E57" s="12"/>
-      <c r="F57" s="11"/>
+      <c r="E57" s="18"/>
+      <c r="F57" s="15"/>
     </row>
     <row r="58" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="8"/>
@@ -1028,7 +1087,7 @@
       <c r="D58" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="E58" s="12"/>
+      <c r="E58" s="16"/>
       <c r="F58" s="11"/>
     </row>
     <row r="59" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1036,16 +1095,16 @@
       <c r="B59" s="6"/>
       <c r="C59" s="6"/>
       <c r="D59" s="9"/>
-      <c r="E59" s="12"/>
-      <c r="F59" s="11"/>
+      <c r="E59" s="17"/>
+      <c r="F59" s="13"/>
     </row>
     <row r="60" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="8"/>
       <c r="B60" s="6"/>
       <c r="C60" s="6"/>
       <c r="D60" s="9"/>
-      <c r="E60" s="12"/>
-      <c r="F60" s="11"/>
+      <c r="E60" s="18"/>
+      <c r="F60" s="15"/>
     </row>
     <row r="61" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="8"/>
@@ -1058,7 +1117,7 @@
       <c r="D61" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="E61" s="12"/>
+      <c r="E61" s="16"/>
       <c r="F61" s="11"/>
     </row>
     <row r="62" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1066,16 +1125,16 @@
       <c r="B62" s="6"/>
       <c r="C62" s="6"/>
       <c r="D62" s="9"/>
-      <c r="E62" s="12"/>
-      <c r="F62" s="11"/>
+      <c r="E62" s="17"/>
+      <c r="F62" s="13"/>
     </row>
     <row r="63" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="8"/>
       <c r="B63" s="6"/>
       <c r="C63" s="6"/>
       <c r="D63" s="9"/>
-      <c r="E63" s="12"/>
-      <c r="F63" s="11"/>
+      <c r="E63" s="18"/>
+      <c r="F63" s="15"/>
     </row>
     <row r="64" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A64" s="8"/>
@@ -1088,7 +1147,7 @@
       <c r="D64" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="E64" s="12"/>
+      <c r="E64" s="16"/>
       <c r="F64" s="11"/>
     </row>
     <row r="65" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1096,16 +1155,16 @@
       <c r="B65" s="6"/>
       <c r="C65" s="6"/>
       <c r="D65" s="9"/>
-      <c r="E65" s="12"/>
-      <c r="F65" s="11"/>
+      <c r="E65" s="17"/>
+      <c r="F65" s="13"/>
     </row>
     <row r="66" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A66" s="8"/>
       <c r="B66" s="6"/>
       <c r="C66" s="6"/>
       <c r="D66" s="9"/>
-      <c r="E66" s="12"/>
-      <c r="F66" s="11"/>
+      <c r="E66" s="18"/>
+      <c r="F66" s="15"/>
     </row>
     <row r="67" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A67" s="8"/>
@@ -1118,7 +1177,7 @@
       <c r="D67" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="E67" s="12"/>
+      <c r="E67" s="16"/>
       <c r="F67" s="11"/>
     </row>
     <row r="68" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1126,16 +1185,16 @@
       <c r="B68" s="6"/>
       <c r="C68" s="6"/>
       <c r="D68" s="9"/>
-      <c r="E68" s="12"/>
-      <c r="F68" s="11"/>
+      <c r="E68" s="17"/>
+      <c r="F68" s="13"/>
     </row>
     <row r="69" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="8"/>
       <c r="B69" s="6"/>
       <c r="C69" s="6"/>
       <c r="D69" s="9"/>
-      <c r="E69" s="12"/>
-      <c r="F69" s="11"/>
+      <c r="E69" s="18"/>
+      <c r="F69" s="15"/>
     </row>
     <row r="70" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A70" s="8"/>
@@ -1148,7 +1207,7 @@
       <c r="D70" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="E70" s="12"/>
+      <c r="E70" s="16"/>
       <c r="F70" s="11"/>
     </row>
     <row r="71" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1156,16 +1215,16 @@
       <c r="B71" s="6"/>
       <c r="C71" s="6"/>
       <c r="D71" s="9"/>
-      <c r="E71" s="12"/>
-      <c r="F71" s="11"/>
+      <c r="E71" s="17"/>
+      <c r="F71" s="13"/>
     </row>
     <row r="72" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A72" s="8"/>
       <c r="B72" s="6"/>
       <c r="C72" s="6"/>
       <c r="D72" s="9"/>
-      <c r="E72" s="12"/>
-      <c r="F72" s="11"/>
+      <c r="E72" s="18"/>
+      <c r="F72" s="15"/>
     </row>
     <row r="73" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A73" s="8"/>
@@ -1178,7 +1237,7 @@
       <c r="D73" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="E73" s="12"/>
+      <c r="E73" s="16"/>
       <c r="F73" s="11"/>
     </row>
     <row r="74" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1186,16 +1245,16 @@
       <c r="B74" s="6"/>
       <c r="C74" s="6"/>
       <c r="D74" s="9"/>
-      <c r="E74" s="12"/>
-      <c r="F74" s="11"/>
+      <c r="E74" s="17"/>
+      <c r="F74" s="13"/>
     </row>
     <row r="75" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A75" s="8"/>
       <c r="B75" s="6"/>
       <c r="C75" s="6"/>
       <c r="D75" s="9"/>
-      <c r="E75" s="12"/>
-      <c r="F75" s="11"/>
+      <c r="E75" s="18"/>
+      <c r="F75" s="15"/>
     </row>
     <row r="76" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A76" s="8"/>
@@ -1208,7 +1267,7 @@
       <c r="D76" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="E76" s="12"/>
+      <c r="E76" s="16"/>
       <c r="F76" s="11"/>
     </row>
     <row r="77" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1216,16 +1275,16 @@
       <c r="B77" s="6"/>
       <c r="C77" s="6"/>
       <c r="D77" s="9"/>
-      <c r="E77" s="12"/>
-      <c r="F77" s="11"/>
+      <c r="E77" s="17"/>
+      <c r="F77" s="13"/>
     </row>
     <row r="78" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A78" s="8"/>
       <c r="B78" s="6"/>
       <c r="C78" s="6"/>
       <c r="D78" s="9"/>
-      <c r="E78" s="12"/>
-      <c r="F78" s="11"/>
+      <c r="E78" s="18"/>
+      <c r="F78" s="15"/>
     </row>
     <row r="79" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A79" s="8"/>
@@ -1238,7 +1297,7 @@
       <c r="D79" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="E79" s="12"/>
+      <c r="E79" s="16"/>
       <c r="F79" s="11"/>
     </row>
     <row r="80" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1246,16 +1305,16 @@
       <c r="B80" s="6"/>
       <c r="C80" s="6"/>
       <c r="D80" s="9"/>
-      <c r="E80" s="12"/>
-      <c r="F80" s="11"/>
+      <c r="E80" s="17"/>
+      <c r="F80" s="13"/>
     </row>
     <row r="81" customFormat="false" ht="64.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A81" s="8"/>
       <c r="B81" s="6"/>
       <c r="C81" s="6"/>
       <c r="D81" s="9"/>
-      <c r="E81" s="12"/>
-      <c r="F81" s="11"/>
+      <c r="E81" s="18"/>
+      <c r="F81" s="15"/>
     </row>
     <row r="82" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A82" s="8"/>
@@ -1268,7 +1327,7 @@
       <c r="D82" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="E82" s="12"/>
+      <c r="E82" s="16"/>
       <c r="F82" s="11"/>
     </row>
     <row r="83" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1276,16 +1335,16 @@
       <c r="B83" s="6"/>
       <c r="C83" s="6"/>
       <c r="D83" s="9"/>
-      <c r="E83" s="12"/>
-      <c r="F83" s="11"/>
+      <c r="E83" s="17"/>
+      <c r="F83" s="13"/>
     </row>
     <row r="84" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A84" s="8"/>
       <c r="B84" s="6"/>
       <c r="C84" s="6"/>
       <c r="D84" s="9"/>
-      <c r="E84" s="12"/>
-      <c r="F84" s="11"/>
+      <c r="E84" s="18"/>
+      <c r="F84" s="15"/>
     </row>
     <row r="85" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A85" s="8"/>
@@ -1298,7 +1357,7 @@
       <c r="D85" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="E85" s="12"/>
+      <c r="E85" s="16"/>
       <c r="F85" s="11"/>
     </row>
     <row r="86" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1306,16 +1365,16 @@
       <c r="B86" s="6"/>
       <c r="C86" s="6"/>
       <c r="D86" s="9"/>
-      <c r="E86" s="12"/>
-      <c r="F86" s="11"/>
+      <c r="E86" s="17"/>
+      <c r="F86" s="13"/>
     </row>
     <row r="87" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A87" s="8"/>
       <c r="B87" s="6"/>
       <c r="C87" s="6"/>
       <c r="D87" s="9"/>
-      <c r="E87" s="12"/>
-      <c r="F87" s="11"/>
+      <c r="E87" s="18"/>
+      <c r="F87" s="15"/>
     </row>
     <row r="88" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A88" s="8"/>
@@ -1328,7 +1387,7 @@
       <c r="D88" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="E88" s="12"/>
+      <c r="E88" s="16"/>
       <c r="F88" s="11"/>
     </row>
     <row r="89" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1336,16 +1395,16 @@
       <c r="B89" s="6"/>
       <c r="C89" s="6"/>
       <c r="D89" s="9"/>
-      <c r="E89" s="12"/>
-      <c r="F89" s="11"/>
+      <c r="E89" s="17"/>
+      <c r="F89" s="13"/>
     </row>
     <row r="90" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A90" s="8"/>
       <c r="B90" s="6"/>
       <c r="C90" s="6"/>
       <c r="D90" s="9"/>
-      <c r="E90" s="12"/>
-      <c r="F90" s="11"/>
+      <c r="E90" s="18"/>
+      <c r="F90" s="15"/>
     </row>
     <row r="91" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A91" s="8"/>
@@ -1358,7 +1417,7 @@
       <c r="D91" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="E91" s="12"/>
+      <c r="E91" s="16"/>
       <c r="F91" s="11"/>
     </row>
     <row r="92" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1366,16 +1425,16 @@
       <c r="B92" s="6"/>
       <c r="C92" s="6"/>
       <c r="D92" s="9"/>
-      <c r="E92" s="12"/>
-      <c r="F92" s="11"/>
+      <c r="E92" s="17"/>
+      <c r="F92" s="13"/>
     </row>
     <row r="93" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A93" s="8"/>
       <c r="B93" s="6"/>
       <c r="C93" s="6"/>
       <c r="D93" s="9"/>
-      <c r="E93" s="12"/>
-      <c r="F93" s="11"/>
+      <c r="E93" s="18"/>
+      <c r="F93" s="15"/>
     </row>
     <row r="94" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A94" s="8"/>
@@ -1388,7 +1447,7 @@
       <c r="D94" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="E94" s="12"/>
+      <c r="E94" s="16"/>
       <c r="F94" s="11"/>
     </row>
     <row r="95" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1396,32 +1455,35 @@
       <c r="B95" s="6"/>
       <c r="C95" s="6"/>
       <c r="D95" s="9"/>
-      <c r="E95" s="12"/>
-      <c r="F95" s="11"/>
+      <c r="E95" s="17"/>
+      <c r="F95" s="13"/>
     </row>
     <row r="96" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A96" s="8"/>
       <c r="B96" s="6"/>
       <c r="C96" s="6"/>
       <c r="D96" s="9"/>
-      <c r="E96" s="12"/>
-      <c r="F96" s="11"/>
+      <c r="E96" s="18"/>
+      <c r="F96" s="15"/>
     </row>
     <row r="97" customFormat="false" ht="26.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B97" s="13"/>
-      <c r="C97" s="13"/>
-      <c r="D97" s="13"/>
+      <c r="B97" s="19"/>
+      <c r="C97" s="19"/>
+      <c r="D97" s="19"/>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B98" s="1"/>
-      <c r="C98" s="1"/>
-      <c r="D98" s="1"/>
-      <c r="F98" s="1"/>
+      <c r="A98" s="20"/>
+      <c r="B98" s="20"/>
+      <c r="C98" s="20"/>
+      <c r="D98" s="20"/>
+      <c r="E98" s="20"/>
+      <c r="F98" s="20"/>
     </row>
   </sheetData>
-  <mergeCells count="127">
+  <mergeCells count="128">
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A2:F2"/>
+    <mergeCell ref="E3:F3"/>
     <mergeCell ref="A4:A6"/>
     <mergeCell ref="B4:B6"/>
     <mergeCell ref="C4:C6"/>
@@ -1549,11 +1611,11 @@
     <mergeCell ref="A98:F98"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="0.253472222222222" bottom="0.709027777777778" header="0.511811023622047" footer="0.44375"/>
+  <pageMargins left="0.7875" right="0.7875" top="0.253472222222222" bottom="0.577083333333333" header="0.511811023622047" footer="0.311805555555556"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
-    <oddFooter>&amp;C&amp;"Times New Roman,Обычный"&amp;12Страница &amp;P</oddFooter>
+    <oddFooter>&amp;L&amp;"Times New Roman,Обычный"&amp;12Ответственный за электрохозяйство по подразделению: &amp;R&amp;"Times New Roman,Обычный"&amp;12&amp;P из &amp;N</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>